<commit_message>
add HtmReporter and EmailAlerter
</commit_message>
<xml_diff>
--- a/src/main/resources/excels-repo.tmpl.xlsx
+++ b/src/main/resources/excels-repo.tmpl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>source</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -430,22 +430,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>global.key1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>global.value1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>global.key2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>global.key3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>global.key4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -459,14 +443,6 @@
   </si>
   <si>
     <t>global.key7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>global.value2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>global.value3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -563,6 +539,34 @@
   <si>
     <t>var code = test_case_context["response.status"];
 Assert.assertTrue(200 == code || 302 == code);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>global.mail_from</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>env_context["global_context"] = global_context;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>global.mail_to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2476382757@qq.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>global.mail_subject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动测试报告</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2476382757@my-home-comp.com</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -639,7 +643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -650,6 +654,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -957,7 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
+    <sheetView topLeftCell="H2" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -987,7 +992,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>7</v>
@@ -999,10 +1004,10 @@
         <v>13</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>8</v>
@@ -1037,10 +1042,10 @@
         <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>30</v>
@@ -1049,7 +1054,7 @@
         <v>29</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="81" x14ac:dyDescent="0.15">
@@ -1072,16 +1077,16 @@
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="81" x14ac:dyDescent="0.15">
@@ -1104,10 +1109,10 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>26</v>
@@ -1119,7 +1124,7 @@
         <v>28</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="81" x14ac:dyDescent="0.15">
@@ -1142,22 +1147,22 @@
         <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="283.5" x14ac:dyDescent="0.15">
@@ -1177,7 +1182,7 @@
         <v>35</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1198,14 +1203,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -1218,62 +1223,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
+        <v>63</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
         <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -1281,15 +1290,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
@@ -1300,6 +1309,11 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1357,7 +1371,7 @@
     </row>
     <row r="2" spans="1:1" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>